<commit_message>
in the process of making an Archi-import for Blik
</commit_message>
<xml_diff>
--- a/Blik/Domeinen.xlsx
+++ b/Blik/Domeinen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="210" windowWidth="12195" windowHeight="6510" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="270" windowWidth="12195" windowHeight="6450"/>
   </bookViews>
   <sheets>
     <sheet name="Domeinen" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="100">
   <si>
     <t>Divisie</t>
   </si>
@@ -282,6 +282,39 @@
   </si>
   <si>
     <t>Bureau Risicobeoordeling en Onderzoeksprogrammering</t>
+  </si>
+  <si>
+    <t>wetgeving</t>
+  </si>
+  <si>
+    <t>BWBR0002458</t>
+  </si>
+  <si>
+    <t>BWBR0002458, BWBR0004302</t>
+  </si>
+  <si>
+    <t>BWBR0003081</t>
+  </si>
+  <si>
+    <t>Wet op de dierproeven</t>
+  </si>
+  <si>
+    <t>Drank- en Horecawet</t>
+  </si>
+  <si>
+    <t>Drank- en Horecawet; Tabakswet</t>
+  </si>
+  <si>
+    <t>BWBR0003818</t>
+  </si>
+  <si>
+    <t>Diergeneesmiddelenwet</t>
+  </si>
+  <si>
+    <t>BWBR0005662</t>
+  </si>
+  <si>
+    <t>Gezondheids- en welzijnswet voor dieren</t>
   </si>
 </sst>
 </file>
@@ -376,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -389,6 +422,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -758,15 +792,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="35.85546875" customWidth="1"/>
+    <col min="4" max="4" width="44.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>56</v>
       </c>
@@ -776,8 +814,11 @@
       <c r="C1" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -788,7 +829,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>55</v>
       </c>
@@ -798,8 +839,14 @@
       <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>54</v>
       </c>
@@ -810,7 +857,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>39</v>
       </c>
@@ -821,7 +868,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>47</v>
       </c>
@@ -832,7 +879,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>37</v>
       </c>
@@ -842,8 +889,14 @@
       <c r="C7" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>46</v>
       </c>
@@ -853,8 +906,14 @@
       <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>53</v>
       </c>
@@ -865,7 +924,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
@@ -875,8 +934,14 @@
       <c r="C10" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>52</v>
       </c>
@@ -887,7 +952,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>45</v>
       </c>
@@ -898,7 +963,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -909,7 +974,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>44</v>
       </c>
@@ -920,7 +985,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>43</v>
       </c>
@@ -931,7 +996,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>42</v>
       </c>
@@ -942,7 +1007,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>51</v>
       </c>
@@ -952,8 +1017,14 @@
       <c r="C17" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>35</v>
       </c>
@@ -964,7 +1035,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>30</v>
       </c>
@@ -975,7 +1046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>34</v>
       </c>
@@ -986,7 +1057,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>41</v>
       </c>
@@ -997,7 +1068,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>50</v>
       </c>
@@ -1008,7 +1079,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>40</v>
       </c>
@@ -1019,7 +1090,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>38</v>
       </c>
@@ -1030,7 +1101,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>49</v>
       </c>
@@ -1041,7 +1112,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>48</v>
       </c>
@@ -1052,7 +1123,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>33</v>
       </c>
@@ -1063,7 +1134,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>60</v>
       </c>
@@ -1083,7 +1154,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>